<commit_message>
docs(report): master cases & AB intuition, initial plots
</commit_message>
<xml_diff>
--- a/plots.xlsx
+++ b/plots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dkapa\Desktop\AITU\DAA\DAA_assignment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DE9213-04FE-4EDC-95A9-B2B51B2F1C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD52298-0306-4705-BD9A-1E7B3BB82149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4484,8 +4484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50E98C3-4F92-47D9-AE17-F13A6C1D2DBD}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="78" workbookViewId="0">
-      <selection activeCell="T18" sqref="T18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="78" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>

</xml_diff>